<commit_message>
sprint-2 class notes and requirements change
</commit_message>
<xml_diff>
--- a/User Stories -v1.xlsx
+++ b/User Stories -v1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
   <si>
     <t xml:space="preserve">S.No </t>
   </si>
@@ -41,12 +41,6 @@
     <t>Design-Create REST API for withdraw an anount</t>
   </si>
   <si>
-    <t>Design-Create REST API for card block /unblock for an account</t>
-  </si>
-  <si>
-    <t>Design-Create REST API for get blocked cards</t>
-  </si>
-  <si>
     <t>Ravi</t>
   </si>
   <si>
@@ -77,12 +71,6 @@
     <t>Develop- REST API for withdraw an anount</t>
   </si>
   <si>
-    <t>Develop- REST API for card block /unblock for an account</t>
-  </si>
-  <si>
-    <t>Develop- REST API for get blocked cards</t>
-  </si>
-  <si>
     <t>Snowflake account creation and databse creation</t>
   </si>
   <si>
@@ -120,9 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements </t>
-  </si>
-  <si>
-    <t>As a developer I want to develop a scheduler flow  using the below requirements it should run at 7PM every day</t>
   </si>
   <si>
     <t>As a developer I want to develop a scheduler flow  using the below requirements it should run at 6PM every day</t>
@@ -150,84 +135,6 @@
     Postman/Thunder client
     7-zip 
 </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/checkBalance : 
-Method : GET 
-queryParams :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bank - required: should be one of enum values ICICI , AXIS , HDFC 
-type - required : should be on of enum values [savings , current] 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Body : json</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- accountNum - required: should be string and min max length is 10 
-atmPin : required : type string (but pass numbers in string) min max length = 4 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sample Response : 200 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- {“status” : “Your total balance is xxxxxxxx as on 20-JAN-2024 is xxxxxx”}
-NOTE: Implement basic security for the API</t>
-    </r>
   </si>
   <si>
     <r>
@@ -593,84 +500,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/withDraw : 
-Method : POST 
-queryParams :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bank - required: should be one of enum values ICICI , AXIS ,HDFC,SBI 
-type - required : should be on of enum values [savings , current] 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Body : json </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-accountNum - required: should be string and min max length is 10
- atmPin : required : type string (but pass numbers in string) min max length = 4 amountToBeWithdraw : Required. it should be number 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sample Response : 200 : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-{“status” : “Amount xxxx is debited . Your total balance is xxxxxxxx”}
-</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">As a developer I want to develop a scheduler flow  using the below requirements it should run at 6PM every day
 Have a scheduler in your application which will trigger a flow daily at 
 6pm where it should fetch the Locked cards and send out individual email to customers and Bank vendors 
@@ -707,133 +536,6 @@
   </si>
   <si>
     <t>Design-Create REST API for withdraw an amount</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/cardUnLock : 
-/cardLock : 
-Method : PUT 
-Body : json </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-user with default value “admin” 
-password with default value “admin” 
-accountNum - required: should be string and min max length is 10 
-bank - required: should be one of enum values ICICI , AXIS , HDFC ,SBI
-type –required: should be one for enum values lock,UnLock
-Sampl
-NOTE: Implement basic security for the API</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-/getBlockedCards : 
-Method : GET </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">queryParams : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-bank - required: should be one of enum values ICICI , AXIS , HDFC 
-type –required: should be one for enum values Block
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sample Response : 200 : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-{ 
-customerName : "ravi",
-bank: "HDFC",
-type - "savings",
-branchName -"BLR",
- accountNum -"54326781234",
- atmPin :"1234",
-ifscCode - "HDFC10034",
-mailId : "ravi@gmail.com",
-cardStatus : "Locked"
-}
-NOTE: Implement basic security for the API</t>
-    </r>
-  </si>
-  <si>
-    <t>Design-Create REST API for get Locked cards</t>
   </si>
   <si>
     <r>
@@ -1117,7 +819,275 @@
     </r>
   </si>
   <si>
-    <t>Develop- REST API for get Locked cards</t>
+    <t>Develop- REST API for card Lock /unLock for an account</t>
+  </si>
+  <si>
+    <t>As a developer I want to develop API based on RAML and based on the below requirements 
+fetch all the Locked cards and display the records in front end</t>
+  </si>
+  <si>
+    <t>As a developer I want to develop a scheduler flow  using the below requirements it should run at 9PM every day</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Develop- REST API for card lock /unlock for an account</t>
+  </si>
+  <si>
+    <t>Develop- REST API for get locked cards</t>
+  </si>
+  <si>
+    <t>InProgress</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/checkBalance : 
+Method : GET 
+queryParams :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bank - required: should be one of enum values ICICI , AXIS , HDFC 
+type - required : should be on of enum values [savings , current] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ accountNum - required: should be string and min max length is 10 
+atmPin : required : type string (but pass numbers in string) min max length = 4 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sample Response : 200 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ {“status” : “Your total balance is xxxxxxxx as on 20-JAN-2024 is xxxxxx”}
+NOTE: Implement basic security for the API</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/withDraw : 
+Method : POST 
+queryParams :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bank - required: should be one of enum values ICICI , AXIS ,HDFC,SBI 
+type - required : should be on of enum values [savings , current] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+accountNum - required: should be string and min max length is 10
+ atmPin : required : type string (but pass numbers in string) min max length = 4 amountToBeWithdraw : Required. it should be number 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sample Response : 200 : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{“status” : “Amount xxxx is debited . Your total balance is xxxxxxxx”}
+</t>
+    </r>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Design-Create REST API for get locked cards</t>
+  </si>
+  <si>
+    <t>Design-Create REST API for get Locked Accounts</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+/getLockedAccts: 
+Method : GET </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">queryParams : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+bank - required: should be one of enum values ICICI , AXIS , HDFC 
+type –required: should be one for enum values Block
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sample Response : 200 : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{ 
+customerName : "ravi",
+bank: "HDFC",
+type - "savings",
+branchName -"BLR",
+ accountNum -"54326781234",
+ atmPin :"1234",
+ifscCode - "HDFC10034",
+mailId : "ravi@gmail.com",
+cardStatus : "Locked"
+}
+NOTE: Implement basic security for the API</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Create batch flow to Send Emails for Locked Accounts </t>
+  </si>
+  <si>
+    <t>Develop- REST API for get Locked Accounts</t>
   </si>
   <si>
     <r>
@@ -1133,40 +1103,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">/unLock : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> /Lock:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-UnLock resource is used to unLock the locked account 
+      <t xml:space="preserve">/AcctLockUnlock : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+AcctLockUnlock resource is used to Lock/ unLock the  account 
  Check if user and password = admin 
 Check if valid combination of bank and Account number is given : 
 • If no, return the response saying “Account 1234567890 does not exist . 
@@ -1229,14 +1177,44 @@
     </r>
   </si>
   <si>
-    <t>Develop- REST API for card Lock /unLock for an account</t>
-  </si>
-  <si>
-    <t>As a developer I want to develop API based on RAML and based on the below requirements 
-fetch all the Locked cards and display the records in front end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create batch flow to Send Emails for Locked cards </t>
+    <r>
+      <t xml:space="preserve">As a developer I want to desing RAML by using the below requirements 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/AcctUnLock : 
+/AcctLock : 
+Method : PUT 
+Body : json </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+user with default value “admin” 
+password with default value “admin” 
+accountNum - required: should be string and min max length is 10 
+bank - required: should be one of enum values ICICI , AXIS , HDFC ,SBI
+type –required: should be one for enum values lock,UnLock
+sample response : 200
+{
+"status": "Your Account- XXXXXXXXXXX With Bank- HDFC  is Unlocked/Locked Now"
+}
+NOTE: Implement basic security for the API</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1281,7 +1259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1291,6 +1269,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1332,6 +1322,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1633,20 +1626,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="52.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="93.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,13 +1648,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1668,13 +1665,16 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1682,13 +1682,16 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1696,13 +1699,16 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1710,206 +1716,230 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
+      <c r="C7" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
+      <c r="C8" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
+      <c r="C13" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
+      <c r="C14" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1922,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1941,13 +1971,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
@@ -1958,10 +1988,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
@@ -1972,13 +2002,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1986,38 +2016,38 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -2025,13 +2055,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="403.2" x14ac:dyDescent="0.3">
@@ -2039,13 +2069,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="216" x14ac:dyDescent="0.3">
@@ -2053,13 +2083,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
@@ -2067,13 +2097,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
@@ -2081,13 +2111,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
@@ -2095,13 +2125,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2109,13 +2139,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2123,13 +2153,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
@@ -2137,13 +2167,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -2151,13 +2181,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -2165,13 +2195,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2195,12 +2225,12 @@
   <sheetData>
     <row r="4" spans="4:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="4:4" ht="242.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2223,37 +2253,37 @@
   <sheetData>
     <row r="5" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E5" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E6" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E7" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E8" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E9" s="9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E10" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E11" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2264,10 +2294,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:D11"/>
+  <dimension ref="C4:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2275,44 +2305,65 @@
     <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:4" ht="18" x14ac:dyDescent="0.3">
       <c r="D4" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="C11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D5" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D6" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D7" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D8" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D9" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D10" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="D11" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>